<commit_message>
precomputed for degree, much faster now
</commit_message>
<xml_diff>
--- a/njs199.xlsx
+++ b/njs199.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sasha/Documents/Classes/EECS 348/Assignment3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Problem</t>
   </si>
@@ -47,6 +57,12 @@
   </si>
   <si>
     <t>number of consistency checks, i.e. variable assignments</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Run on the easy board, average of ten trials</t>
   </si>
 </sst>
 </file>
@@ -147,9 +163,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -182,9 +198,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -391,21 +407,22 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56" customWidth="1"/>
     <col min="8" max="8" width="44.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,26 +441,47 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
       <c r="H1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>

</xml_diff>